<commit_message>
added loading .gif functnality while page gets rendered
</commit_message>
<xml_diff>
--- a/Documents/reviews_url1.xlsx
+++ b/Documents/reviews_url1.xlsx
@@ -444,9 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Dont buy.. after 10 to.15 mins gaming phone lagging too much
-</t>
+          <t>best camera and display and best performance in the  segment ..... excellent for gaming... pubg experiece is so perfect and the g95 processor gives a best performance</t>
         </is>
       </c>
     </row>
@@ -456,9 +454,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Good phoneDecent look and looks stylishCamera and battery quality are super goodGood phone in this range 👍But delivery service is not good
-</t>
+          <t>When we talk about a brand loyal person....so here i am....it is pleasure to say that...you are coming to a very superb brand which was already known by Realme....this Realme 7 in mist blue colour is awesome as well as their performance is un-beatable....i mean wow yr.....this hand-set is having a different personality when it was carried whether inside the house or outside in a party or wedding function....what a wonderful performance bro....💓So i prerer you to purchase this phone....and i...</t>
         </is>
       </c>
     </row>
@@ -468,9 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Not good phone stopped working after some time so i didn't suggest you this...
-</t>
+          <t>Writting this after using for 1 month.Pros.1. Camera is too good at this price range. 2. Compact design (Easily usable in one hand).3. No heavy bloatware installed other than some realme apps.4. Battery durability is quite good.5. No heating issue found even after playing PUBG for 3 hours.Cons.1. Sometimes photos are over exposed. Camera software optimization needs to be improved.2. Sound quality is disappointing3. Display brightness is not enough for a sunny day. You'll get trouble...</t>
         </is>
       </c>
     </row>
@@ -480,9 +474,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Worst product, not as expected its not even a month and ut hangs so much! Its front camera is just worst, only it's first look is good nothing else. Don't go for it!! Redmi note 8 and even note 5 is much better than it!😤 Completely disappointed 😤😤😤
-</t>
+          <t>Best phone in the range Camera is better ✔️Battery backup is ok 👍Fast charging 💯Look is mustPerfomence good ⛹️Aal is very good</t>
         </is>
       </c>
     </row>
@@ -492,9 +484,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Here my product review after usage of 3 months.Cons:If you bought this mobile you can't exchange. I have tried but not able to exchange my device.Please check by clicking the exchange option and you can take the decision.Now you can understand why you should not by this mobile.Gaming - Mobile heating and lagging when you playing high graphics gameBattery - 5020mAh battery. Moderate performFor charging it's take 2.4 hrs per day from 0 to 100.Macro camera - useless featureFront and Rear camera - Not good compare with realme 6000rs mobile camera.UI is fine but consuming more ramMany pre-installed application could not able to delete ( Mi app).I suggest please buy some other brand don't waste your money like me.
-</t>
+          <t>Realme7 It's a branded mobile To value of money and good battery backup Display was awesomeSound quality was nice Good gaming 👍 Camera was extremely super good quality pics Side fingerprint sensor was NYC and speed front camera super Worth for maney No lag no struck 30watts charger was super</t>
         </is>
       </c>
     </row>
@@ -504,9 +494,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Totally impressed by the built and looks. For 13k I thought of getting realme 6i but the stocks barely last..!So I decided to get this phone. The phone is great and smooth. Gaming experience is also good but not as good as g90t.G85 is a decent processor with great daily life performance!If 12k is your budget go for it..Or 13k..realme 6i and 14k... Go for poco m2. Scarlet red looks stunning!!
-</t>
+          <t>GooD d AsomE Mobile, Battery  was so gooD and fast charge   i love this phonE camera was so nicE</t>
         </is>
       </c>
     </row>
@@ -516,9 +504,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Awesome product 💎Value for money 💵Best in segment📱For normal usage this one is the best 🙌Long battery life 🤳 when compared to other smartphones.Camera is ok for this price📸Charging is comparitively slow it takes 2 - 2 and half hrs or more to get full charged.🕕 Overall its best for the price  👍
-</t>
+          <t>Good value for money and a phone with good camera and great battery life with fast charging which is a life saver sometimes</t>
         </is>
       </c>
     </row>
@@ -528,9 +514,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Very nice Phone.. smooth performance.. charge service decent.. screen quality superb.. sound ok.. but body vibration issue is here.. in speaker mode or at time of calling body vibration present.. no notification light.. overall decent performance at this price.. phone support only 18 watt fast charge. But charger support 22.5 watt..
-</t>
+          <t>Best mobile ...very good camera quality ... Fast refresh rate... Value of money.. must enjoyed this mobile</t>
         </is>
       </c>
     </row>
@@ -540,9 +524,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  My Mobile phone has some screen issue. On completely black wall paper or black background there's a permanent white dot (like screen is defective) on the screen but i requested for the replacement soon device will be replaced. Although device is preety average, ram management is not that good.go for the snapdragon rather than mediatek.Pubg lags sometimes on medium settings and there's a ton of preloaded apps from which some apps you cannot uninstall.there are several options in the market other than xiaomi. So,choose your device wisely.
-</t>
+          <t>I overall like this phone. Good performance, camera, battery is also better not so high. Still I am satisfied with the phone</t>
         </is>
       </c>
     </row>
@@ -552,9 +534,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-  Hi I am writing this review post usage of 7 days,1. The Dsiplay is perfect better than Samsung M21 in the similar price range. The display is Full HD+ whereas its counter parts are not offering that.2. The camera scores over its counter parts whereas not much variations available in Selfie but fantastic at this price.3. The specifications are more or less similar to Mi Note 8 except the processor, it's Helios G85 in this one whereas its Qualcomm in Note 8 i.e 625.4. Note 8 had 4K video capture option but not with the latest  Note 9.5. The battery stays long as promised as I am not a gamer the battery lasts for over a day and half.6. This had P2i protection towards splash but not with Note 8.7. To conclude I shall recommend this phone as no brands available at such good price.Thanks for reading god bless . Enjoy
-</t>
+          <t>Very awesome mobile. Camera is good but front camera is not that much better. Overall it is better than samsung M21 or M31 if you are planning for these smartphones so change your desigen and buy Realme 7. Charging is tooo good.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Done and tested for flipkart site
</commit_message>
<xml_diff>
--- a/Documents/reviews_url1.xlsx
+++ b/Documents/reviews_url1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,106 +438,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>best camera and display and best performance in the  segment ..... excellent for gaming... pubg experiece is so perfect and the g95 processor gives a best performance</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>When we talk about a brand loyal person....so here i am....it is pleasure to say that...you are coming to a very superb brand which was already known by Realme....this Realme 7 in mist blue colour is awesome as well as their performance is un-beatable....i mean wow yr.....this hand-set is having a different personality when it was carried whether inside the house or outside in a party or wedding function....what a wonderful performance bro....💓So i prerer you to purchase this phone....and i...</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Writting this after using for 1 month.Pros.1. Camera is too good at this price range. 2. Compact design (Easily usable in one hand).3. No heavy bloatware installed other than some realme apps.4. Battery durability is quite good.5. No heating issue found even after playing PUBG for 3 hours.Cons.1. Sometimes photos are over exposed. Camera software optimization needs to be improved.2. Sound quality is disappointing3. Display brightness is not enough for a sunny day. You'll get trouble...</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Best phone in the range Camera is better ✔️Battery backup is ok 👍Fast charging 💯Look is mustPerfomence good ⛹️Aal is very good</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Realme7 It's a branded mobile To value of money and good battery backup Display was awesomeSound quality was nice Good gaming 👍 Camera was extremely super good quality pics Side fingerprint sensor was NYC and speed front camera super Worth for maney No lag no struck 30watts charger was super</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>GooD d AsomE Mobile, Battery  was so gooD and fast charge   i love this phonE camera was so nicE</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Good value for money and a phone with good camera and great battery life with fast charging which is a life saver sometimes</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Best mobile ...very good camera quality ... Fast refresh rate... Value of money.. must enjoyed this mobile</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>I overall like this phone. Good performance, camera, battery is also better not so high. Still I am satisfied with the phone</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Very awesome mobile. Camera is good but front camera is not that much better. Overall it is better than samsung M21 or M31 if you are planning for these smartphones so change your desigen and buy Realme 7. Charging is tooo good.</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>